<commit_message>
updated look and feel
</commit_message>
<xml_diff>
--- a/WeddingBudget.xlsx
+++ b/WeddingBudget.xlsx
@@ -9,16 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="SutterBudget">Sheet1!$B$2</definedName>
+    <definedName name="SutterContribution">Sheet1!$B$2</definedName>
     <definedName name="TotalBudget">Sheet1!$B$4</definedName>
-    <definedName name="TotalExpenses">Sheet1!$B$5</definedName>
+    <definedName name="TotalContribution">Sheet1!$B$4</definedName>
+    <definedName name="TotalExpenses">Sheet1!$B$6</definedName>
     <definedName name="WilkeningBudget">Sheet1!$B$3</definedName>
+    <definedName name="WilkeningContribution">Sheet1!$B$3</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Sutters</t>
-  </si>
-  <si>
-    <t>Wilkenings</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Simply Ballroom Downpayment</t>
   </si>
@@ -47,15 +44,6 @@
     <t>Wedding Payments</t>
   </si>
   <si>
-    <t>Sutter Budget</t>
-  </si>
-  <si>
-    <t>Wilkening Budget</t>
-  </si>
-  <si>
-    <t>Total Budget</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -78,6 +66,30 @@
   </si>
   <si>
     <t>Evy shipping</t>
+  </si>
+  <si>
+    <t>Photographer DownPayment</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Sutter Contribution</t>
+  </si>
+  <si>
+    <t>Wilkening Contribution</t>
+  </si>
+  <si>
+    <t>Total Contribution</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Anticipated Remaining</t>
+  </si>
+  <si>
+    <t>Photographer Downpayment</t>
   </si>
 </sst>
 </file>
@@ -87,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +126,28 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,11 +215,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -208,19 +254,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SutterExpenses" displayName="SutterExpenses" ref="A12:B40" totalsRowShown="0">
-  <autoFilter ref="A12:B40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Sutters" displayName="Sutters" ref="D13:E41" totalsRowShown="0">
+  <autoFilter ref="D13:E41"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Description"/>
+    <tableColumn id="2" name="Amount" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Wilkenings" displayName="Wilkenings" ref="G13:H41" totalsRowShown="0">
+  <autoFilter ref="G13:H41"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Description" dataDxfId="3"/>
     <tableColumn id="2" name="Amount" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="WilkeningExpenses" displayName="WilkeningExpenses" ref="D12:E40" totalsRowShown="0">
-  <autoFilter ref="D12:E40"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Expenses" displayName="Expenses" ref="A13:B41" totalsRowShown="0">
+  <autoFilter ref="A13:B41"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Description" dataDxfId="1"/>
     <tableColumn id="2" name="Amount" dataDxfId="0"/>
@@ -492,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,215 +562,356 @@
     <col min="3" max="3" width="2.5" customWidth="1"/>
     <col min="4" max="4" width="38.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="2.5" customWidth="1"/>
+    <col min="7" max="7" width="38.5" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <f>SUM(Sutters[Amount])</f>
+        <v>200</v>
+      </c>
+      <c r="D2" s="10">
+        <f>7500-SutterBudget</f>
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="10">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <f>SUM(Wilkenings[Amount])</f>
+        <v>550</v>
+      </c>
+      <c r="D3" s="10">
+        <f>7500-WilkeningBudget</f>
+        <v>6950</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B4" s="10">
         <f>SUM(SutterBudget,WilkeningBudget)</f>
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10">
-        <f>SUM(SutterExpenses[Amount],WilkeningExpenses[Amount])</f>
-        <v>296.48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10">
+        <f>SUM(Expenses[Amount])</f>
+        <v>796.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
         <f>TotalBudget-TotalExpenses</f>
-        <v>14703.52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
+        <v>-46.480000000000018</v>
+      </c>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="16"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="D10" s="13"/>
       <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="G10" s="13"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="17"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="G12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E14" s="4">
+        <v>200</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="H14" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4">
+        <v>200</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B16" s="4">
+        <v>5.34</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="4">
-        <v>200</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4">
-        <v>5.34</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="B17" s="4">
         <v>20.7</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="D17"/>
+      <c r="E17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4">
         <v>20.440000000000001</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="D18"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>500</v>
+      </c>
+      <c r="D19"/>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="D20"/>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="D21"/>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="D22"/>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="D23"/>
       <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="D24"/>
       <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="D25"/>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="D26"/>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="D27"/>
       <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="D28"/>
       <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="D29"/>
       <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="D30"/>
       <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
+      <c r="D31"/>
       <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+      <c r="D32"/>
       <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="D33"/>
       <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="D34"/>
       <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="D35"/>
       <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="D36"/>
       <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="D37"/>
       <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="D38"/>
       <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="D39"/>
       <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="D40"/>
       <c r="E40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="D41"/>
+      <c r="E41" s="4"/>
+      <c r="H41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>